<commit_message>
Elvis has left the building. GameOver.
</commit_message>
<xml_diff>
--- a/Documents/Submission_3.0_C13G2/GROUP/SudokuDLX.xlsx
+++ b/Documents/Submission_3.0_C13G2/GROUP/SudokuDLX.xlsx
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="35">
   <si>
     <t>R1C1Z1</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>4x4</t>
+  </si>
+  <si>
+    <t>Note :</t>
+  </si>
+  <si>
+    <t>The above is a representation of a 4x4 matrix. The numbers in the cell correspond to the 16 'Cells' shown in the first colum in the left table. The color schemes for the rows , columns and zones are in direct correspondence to the color schems for the corresponding row, column and zone in the table in the left. For eg. Take Cell no. 10. Its number is 10 and refers to Cell no.10, its column is C3 with shade a medium purple corresponds to C3 shown in the table in the left and the same for Row, R2 in which this cell lies and the zone, Z2, the zone in which it lies.</t>
   </si>
 </sst>
 </file>
@@ -976,7 +982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="256">
+  <cellXfs count="257">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1186,72 +1192,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1326,6 +1266,75 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1627,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BS67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BR16" sqref="BR16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BR26" sqref="BR26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1647,152 +1656,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="15.75" thickBot="1">
-      <c r="C1" s="228" t="s">
+      <c r="C1" s="239" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="229"/>
-      <c r="E1" s="229"/>
-      <c r="F1" s="229"/>
-      <c r="G1" s="229"/>
-      <c r="H1" s="229"/>
-      <c r="I1" s="229"/>
-      <c r="J1" s="229"/>
-      <c r="K1" s="229"/>
-      <c r="L1" s="229"/>
-      <c r="M1" s="229"/>
-      <c r="N1" s="229"/>
-      <c r="O1" s="229"/>
-      <c r="P1" s="229"/>
-      <c r="Q1" s="229"/>
-      <c r="R1" s="230"/>
-      <c r="S1" s="209" t="s">
-        <v>1</v>
-      </c>
-      <c r="T1" s="210"/>
-      <c r="U1" s="210"/>
-      <c r="V1" s="210"/>
-      <c r="W1" s="210"/>
-      <c r="X1" s="210"/>
-      <c r="Y1" s="210"/>
-      <c r="Z1" s="210"/>
-      <c r="AA1" s="210"/>
-      <c r="AB1" s="210"/>
-      <c r="AC1" s="210"/>
-      <c r="AD1" s="210"/>
-      <c r="AE1" s="210"/>
-      <c r="AF1" s="210"/>
-      <c r="AG1" s="210"/>
-      <c r="AH1" s="210"/>
-      <c r="AI1" s="211" t="s">
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
+      <c r="F1" s="240"/>
+      <c r="G1" s="240"/>
+      <c r="H1" s="240"/>
+      <c r="I1" s="240"/>
+      <c r="J1" s="240"/>
+      <c r="K1" s="240"/>
+      <c r="L1" s="240"/>
+      <c r="M1" s="240"/>
+      <c r="N1" s="240"/>
+      <c r="O1" s="240"/>
+      <c r="P1" s="240"/>
+      <c r="Q1" s="240"/>
+      <c r="R1" s="241"/>
+      <c r="S1" s="234" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" s="235"/>
+      <c r="U1" s="235"/>
+      <c r="V1" s="235"/>
+      <c r="W1" s="235"/>
+      <c r="X1" s="235"/>
+      <c r="Y1" s="235"/>
+      <c r="Z1" s="235"/>
+      <c r="AA1" s="235"/>
+      <c r="AB1" s="235"/>
+      <c r="AC1" s="235"/>
+      <c r="AD1" s="235"/>
+      <c r="AE1" s="235"/>
+      <c r="AF1" s="235"/>
+      <c r="AG1" s="235"/>
+      <c r="AH1" s="235"/>
+      <c r="AI1" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="AJ1" s="211"/>
-      <c r="AK1" s="211"/>
-      <c r="AL1" s="211"/>
-      <c r="AM1" s="211"/>
-      <c r="AN1" s="211"/>
-      <c r="AO1" s="211"/>
-      <c r="AP1" s="211"/>
-      <c r="AQ1" s="211"/>
-      <c r="AR1" s="211"/>
-      <c r="AS1" s="211"/>
-      <c r="AT1" s="211"/>
-      <c r="AU1" s="211"/>
-      <c r="AV1" s="211"/>
-      <c r="AW1" s="211"/>
-      <c r="AX1" s="211"/>
-      <c r="AY1" s="212" t="s">
+      <c r="AJ1" s="236"/>
+      <c r="AK1" s="236"/>
+      <c r="AL1" s="236"/>
+      <c r="AM1" s="236"/>
+      <c r="AN1" s="236"/>
+      <c r="AO1" s="236"/>
+      <c r="AP1" s="236"/>
+      <c r="AQ1" s="236"/>
+      <c r="AR1" s="236"/>
+      <c r="AS1" s="236"/>
+      <c r="AT1" s="236"/>
+      <c r="AU1" s="236"/>
+      <c r="AV1" s="236"/>
+      <c r="AW1" s="236"/>
+      <c r="AX1" s="236"/>
+      <c r="AY1" s="237" t="s">
         <v>3</v>
       </c>
-      <c r="AZ1" s="212"/>
-      <c r="BA1" s="212"/>
-      <c r="BB1" s="212"/>
-      <c r="BC1" s="212"/>
-      <c r="BD1" s="212"/>
-      <c r="BE1" s="212"/>
-      <c r="BF1" s="212"/>
-      <c r="BG1" s="212"/>
-      <c r="BH1" s="212"/>
-      <c r="BI1" s="212"/>
-      <c r="BJ1" s="212"/>
-      <c r="BK1" s="212"/>
-      <c r="BL1" s="212"/>
-      <c r="BM1" s="212"/>
-      <c r="BN1" s="213"/>
+      <c r="AZ1" s="237"/>
+      <c r="BA1" s="237"/>
+      <c r="BB1" s="237"/>
+      <c r="BC1" s="237"/>
+      <c r="BD1" s="237"/>
+      <c r="BE1" s="237"/>
+      <c r="BF1" s="237"/>
+      <c r="BG1" s="237"/>
+      <c r="BH1" s="237"/>
+      <c r="BI1" s="237"/>
+      <c r="BJ1" s="237"/>
+      <c r="BK1" s="237"/>
+      <c r="BL1" s="237"/>
+      <c r="BM1" s="237"/>
+      <c r="BN1" s="238"/>
     </row>
     <row r="2" spans="1:71" ht="15.75" thickBot="1">
-      <c r="S2" s="214" t="s">
+      <c r="S2" s="249" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="215"/>
-      <c r="U2" s="215"/>
-      <c r="V2" s="215"/>
-      <c r="W2" s="216" t="s">
+      <c r="T2" s="250"/>
+      <c r="U2" s="250"/>
+      <c r="V2" s="250"/>
+      <c r="W2" s="251" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="216"/>
-      <c r="Y2" s="216"/>
-      <c r="Z2" s="216"/>
-      <c r="AA2" s="217" t="s">
+      <c r="X2" s="251"/>
+      <c r="Y2" s="251"/>
+      <c r="Z2" s="251"/>
+      <c r="AA2" s="252" t="s">
         <v>22</v>
       </c>
-      <c r="AB2" s="217"/>
-      <c r="AC2" s="217"/>
-      <c r="AD2" s="217"/>
-      <c r="AE2" s="218" t="s">
+      <c r="AB2" s="252"/>
+      <c r="AC2" s="252"/>
+      <c r="AD2" s="252"/>
+      <c r="AE2" s="253" t="s">
         <v>23</v>
       </c>
-      <c r="AF2" s="218"/>
-      <c r="AG2" s="218"/>
-      <c r="AH2" s="218"/>
-      <c r="AI2" s="219" t="s">
+      <c r="AF2" s="253"/>
+      <c r="AG2" s="253"/>
+      <c r="AH2" s="253"/>
+      <c r="AI2" s="254" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="219"/>
-      <c r="AK2" s="219"/>
-      <c r="AL2" s="219"/>
-      <c r="AM2" s="220" t="s">
+      <c r="AJ2" s="254"/>
+      <c r="AK2" s="254"/>
+      <c r="AL2" s="254"/>
+      <c r="AM2" s="255" t="s">
         <v>25</v>
       </c>
-      <c r="AN2" s="220"/>
-      <c r="AO2" s="220"/>
-      <c r="AP2" s="220"/>
-      <c r="AQ2" s="221" t="s">
+      <c r="AN2" s="255"/>
+      <c r="AO2" s="255"/>
+      <c r="AP2" s="255"/>
+      <c r="AQ2" s="242" t="s">
         <v>26</v>
       </c>
-      <c r="AR2" s="221"/>
-      <c r="AS2" s="221"/>
-      <c r="AT2" s="221"/>
-      <c r="AU2" s="222" t="s">
+      <c r="AR2" s="242"/>
+      <c r="AS2" s="242"/>
+      <c r="AT2" s="242"/>
+      <c r="AU2" s="243" t="s">
         <v>27</v>
       </c>
-      <c r="AV2" s="222"/>
-      <c r="AW2" s="222"/>
-      <c r="AX2" s="222"/>
-      <c r="AY2" s="223" t="s">
+      <c r="AV2" s="243"/>
+      <c r="AW2" s="243"/>
+      <c r="AX2" s="243"/>
+      <c r="AY2" s="244" t="s">
         <v>28</v>
       </c>
-      <c r="AZ2" s="223"/>
-      <c r="BA2" s="223"/>
-      <c r="BB2" s="223"/>
-      <c r="BC2" s="224" t="s">
+      <c r="AZ2" s="244"/>
+      <c r="BA2" s="244"/>
+      <c r="BB2" s="244"/>
+      <c r="BC2" s="245" t="s">
         <v>29</v>
       </c>
-      <c r="BD2" s="224"/>
-      <c r="BE2" s="224"/>
-      <c r="BF2" s="224"/>
-      <c r="BG2" s="225" t="s">
+      <c r="BD2" s="245"/>
+      <c r="BE2" s="245"/>
+      <c r="BF2" s="245"/>
+      <c r="BG2" s="246" t="s">
         <v>30</v>
       </c>
-      <c r="BH2" s="225"/>
-      <c r="BI2" s="225"/>
-      <c r="BJ2" s="225"/>
-      <c r="BK2" s="226" t="s">
+      <c r="BH2" s="246"/>
+      <c r="BI2" s="246"/>
+      <c r="BJ2" s="246"/>
+      <c r="BK2" s="247" t="s">
         <v>31</v>
       </c>
-      <c r="BL2" s="226"/>
-      <c r="BM2" s="226"/>
-      <c r="BN2" s="227"/>
+      <c r="BL2" s="247"/>
+      <c r="BM2" s="247"/>
+      <c r="BN2" s="248"/>
     </row>
     <row r="3" spans="1:71" ht="15.75" thickBot="1">
       <c r="C3" s="110">
@@ -1987,19 +1996,19 @@
       <c r="BN3" s="89">
         <v>4</v>
       </c>
-      <c r="BO3" s="255" t="s">
+      <c r="BO3" s="233" t="s">
         <v>32</v>
       </c>
-      <c r="BP3" s="253" t="s">
+      <c r="BP3" s="231" t="s">
         <v>24</v>
       </c>
-      <c r="BQ3" s="250" t="s">
+      <c r="BQ3" s="228" t="s">
         <v>25</v>
       </c>
-      <c r="BR3" s="251" t="s">
+      <c r="BR3" s="229" t="s">
         <v>26</v>
       </c>
-      <c r="BS3" s="252" t="s">
+      <c r="BS3" s="230" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2202,19 +2211,19 @@
       <c r="BN4" s="64">
         <v>0</v>
       </c>
-      <c r="BO4" s="254" t="s">
+      <c r="BO4" s="232" t="s">
         <v>20</v>
       </c>
-      <c r="BP4" s="231">
-        <v>1</v>
-      </c>
-      <c r="BQ4" s="232">
+      <c r="BP4" s="209">
+        <v>1</v>
+      </c>
+      <c r="BQ4" s="210">
         <v>5</v>
       </c>
-      <c r="BR4" s="233">
+      <c r="BR4" s="211">
         <v>9</v>
       </c>
-      <c r="BS4" s="234">
+      <c r="BS4" s="212">
         <v>13</v>
       </c>
     </row>
@@ -2417,19 +2426,19 @@
       <c r="BN5" s="65">
         <v>0</v>
       </c>
-      <c r="BO5" s="247" t="s">
+      <c r="BO5" s="225" t="s">
         <v>21</v>
       </c>
-      <c r="BP5" s="235">
+      <c r="BP5" s="213">
         <v>2</v>
       </c>
-      <c r="BQ5" s="236">
+      <c r="BQ5" s="214">
         <v>6</v>
       </c>
-      <c r="BR5" s="237">
+      <c r="BR5" s="215">
         <v>10</v>
       </c>
-      <c r="BS5" s="238">
+      <c r="BS5" s="216">
         <v>14</v>
       </c>
     </row>
@@ -2632,19 +2641,19 @@
       <c r="BN6" s="65">
         <v>0</v>
       </c>
-      <c r="BO6" s="248" t="s">
+      <c r="BO6" s="226" t="s">
         <v>22</v>
       </c>
-      <c r="BP6" s="239">
+      <c r="BP6" s="217">
         <v>3</v>
       </c>
-      <c r="BQ6" s="240">
+      <c r="BQ6" s="218">
         <v>7</v>
       </c>
-      <c r="BR6" s="241">
+      <c r="BR6" s="219">
         <v>11</v>
       </c>
-      <c r="BS6" s="242">
+      <c r="BS6" s="220">
         <v>15</v>
       </c>
     </row>
@@ -2847,19 +2856,19 @@
       <c r="BN7" s="66">
         <v>0</v>
       </c>
-      <c r="BO7" s="249" t="s">
+      <c r="BO7" s="227" t="s">
         <v>23</v>
       </c>
-      <c r="BP7" s="243">
+      <c r="BP7" s="221">
         <v>4</v>
       </c>
-      <c r="BQ7" s="244">
+      <c r="BQ7" s="222">
         <v>8</v>
       </c>
-      <c r="BR7" s="245">
+      <c r="BR7" s="223">
         <v>12</v>
       </c>
-      <c r="BS7" s="246">
+      <c r="BS7" s="224">
         <v>16</v>
       </c>
     </row>
@@ -3262,6 +3271,15 @@
       <c r="BN9" s="71">
         <v>0</v>
       </c>
+      <c r="BO9" t="s">
+        <v>33</v>
+      </c>
+      <c r="BP9" s="256" t="s">
+        <v>34</v>
+      </c>
+      <c r="BQ9" s="256"/>
+      <c r="BR9" s="256"/>
+      <c r="BS9" s="256"/>
     </row>
     <row r="10" spans="1:71" ht="15.75" thickBot="1">
       <c r="A10" s="94">
@@ -3462,6 +3480,10 @@
       <c r="BN10" s="71">
         <v>0</v>
       </c>
+      <c r="BP10" s="256"/>
+      <c r="BQ10" s="256"/>
+      <c r="BR10" s="256"/>
+      <c r="BS10" s="256"/>
     </row>
     <row r="11" spans="1:71" ht="15.75" thickBot="1">
       <c r="A11" s="95">
@@ -3662,6 +3684,10 @@
       <c r="BN11" s="72">
         <v>0</v>
       </c>
+      <c r="BP11" s="256"/>
+      <c r="BQ11" s="256"/>
+      <c r="BR11" s="256"/>
+      <c r="BS11" s="256"/>
     </row>
     <row r="12" spans="1:71" ht="15.75" thickBot="1">
       <c r="A12" s="92">
@@ -3862,6 +3888,10 @@
       <c r="BN12" s="70">
         <v>0</v>
       </c>
+      <c r="BP12" s="256"/>
+      <c r="BQ12" s="256"/>
+      <c r="BR12" s="256"/>
+      <c r="BS12" s="256"/>
     </row>
     <row r="13" spans="1:71" ht="15.75" thickBot="1">
       <c r="A13" s="93">
@@ -4062,6 +4092,10 @@
       <c r="BN13" s="71">
         <v>0</v>
       </c>
+      <c r="BP13" s="256"/>
+      <c r="BQ13" s="256"/>
+      <c r="BR13" s="256"/>
+      <c r="BS13" s="256"/>
     </row>
     <row r="14" spans="1:71" ht="15.75" thickBot="1">
       <c r="A14" s="94">
@@ -4262,6 +4296,10 @@
       <c r="BN14" s="71">
         <v>0</v>
       </c>
+      <c r="BP14" s="256"/>
+      <c r="BQ14" s="256"/>
+      <c r="BR14" s="256"/>
+      <c r="BS14" s="256"/>
     </row>
     <row r="15" spans="1:71" ht="15.75" thickBot="1">
       <c r="A15" s="95">
@@ -4462,6 +4500,10 @@
       <c r="BN15" s="72">
         <v>0</v>
       </c>
+      <c r="BP15" s="256"/>
+      <c r="BQ15" s="256"/>
+      <c r="BR15" s="256"/>
+      <c r="BS15" s="256"/>
     </row>
     <row r="16" spans="1:71" ht="15.75" thickBot="1">
       <c r="A16" s="92">
@@ -4662,8 +4704,12 @@
       <c r="BN16" s="70">
         <v>0</v>
       </c>
+      <c r="BP16" s="256"/>
+      <c r="BQ16" s="256"/>
+      <c r="BR16" s="256"/>
+      <c r="BS16" s="256"/>
     </row>
-    <row r="17" spans="1:66" ht="15.75" thickBot="1">
+    <row r="17" spans="1:71" ht="15.75" thickBot="1">
       <c r="A17" s="93">
         <v>2</v>
       </c>
@@ -4862,8 +4908,12 @@
       <c r="BN17" s="71">
         <v>0</v>
       </c>
+      <c r="BP17" s="256"/>
+      <c r="BQ17" s="256"/>
+      <c r="BR17" s="256"/>
+      <c r="BS17" s="256"/>
     </row>
-    <row r="18" spans="1:66" ht="15.75" thickBot="1">
+    <row r="18" spans="1:71" ht="15.75" thickBot="1">
       <c r="A18" s="94">
         <v>3</v>
       </c>
@@ -5062,8 +5112,12 @@
       <c r="BN18" s="71">
         <v>0</v>
       </c>
+      <c r="BP18" s="256"/>
+      <c r="BQ18" s="256"/>
+      <c r="BR18" s="256"/>
+      <c r="BS18" s="256"/>
     </row>
-    <row r="19" spans="1:66" ht="15.75" thickBot="1">
+    <row r="19" spans="1:71" ht="15.75" thickBot="1">
       <c r="A19" s="95">
         <v>4</v>
       </c>
@@ -5262,8 +5316,12 @@
       <c r="BN19" s="72">
         <v>0</v>
       </c>
+      <c r="BP19" s="256"/>
+      <c r="BQ19" s="256"/>
+      <c r="BR19" s="256"/>
+      <c r="BS19" s="256"/>
     </row>
-    <row r="20" spans="1:66" ht="15.75" thickBot="1">
+    <row r="20" spans="1:71" ht="15.75" thickBot="1">
       <c r="A20" s="92">
         <v>1</v>
       </c>
@@ -5462,8 +5520,12 @@
       <c r="BN20" s="70">
         <v>0</v>
       </c>
+      <c r="BP20" s="256"/>
+      <c r="BQ20" s="256"/>
+      <c r="BR20" s="256"/>
+      <c r="BS20" s="256"/>
     </row>
-    <row r="21" spans="1:66" ht="15.75" thickBot="1">
+    <row r="21" spans="1:71" ht="15.75" thickBot="1">
       <c r="A21" s="93">
         <v>2</v>
       </c>
@@ -5662,8 +5724,12 @@
       <c r="BN21" s="71">
         <v>0</v>
       </c>
+      <c r="BP21" s="256"/>
+      <c r="BQ21" s="256"/>
+      <c r="BR21" s="256"/>
+      <c r="BS21" s="256"/>
     </row>
-    <row r="22" spans="1:66" ht="15.75" thickBot="1">
+    <row r="22" spans="1:71" ht="15.75" thickBot="1">
       <c r="A22" s="94">
         <v>3</v>
       </c>
@@ -5862,8 +5928,12 @@
       <c r="BN22" s="71">
         <v>0</v>
       </c>
+      <c r="BP22" s="256"/>
+      <c r="BQ22" s="256"/>
+      <c r="BR22" s="256"/>
+      <c r="BS22" s="256"/>
     </row>
-    <row r="23" spans="1:66" ht="15.75" thickBot="1">
+    <row r="23" spans="1:71" ht="15.75" thickBot="1">
       <c r="A23" s="95">
         <v>4</v>
       </c>
@@ -6062,8 +6132,12 @@
       <c r="BN23" s="72">
         <v>0</v>
       </c>
+      <c r="BP23" s="256"/>
+      <c r="BQ23" s="256"/>
+      <c r="BR23" s="256"/>
+      <c r="BS23" s="256"/>
     </row>
-    <row r="24" spans="1:66" ht="15.75" thickBot="1">
+    <row r="24" spans="1:71" ht="15.75" thickBot="1">
       <c r="A24" s="92">
         <v>1</v>
       </c>
@@ -6262,8 +6336,12 @@
       <c r="BN24" s="70">
         <v>0</v>
       </c>
+      <c r="BP24" s="256"/>
+      <c r="BQ24" s="256"/>
+      <c r="BR24" s="256"/>
+      <c r="BS24" s="256"/>
     </row>
-    <row r="25" spans="1:66" ht="15.75" thickBot="1">
+    <row r="25" spans="1:71" ht="15.75" thickBot="1">
       <c r="A25" s="93">
         <v>2</v>
       </c>
@@ -6462,8 +6540,12 @@
       <c r="BN25" s="71">
         <v>0</v>
       </c>
+      <c r="BP25" s="256"/>
+      <c r="BQ25" s="256"/>
+      <c r="BR25" s="256"/>
+      <c r="BS25" s="256"/>
     </row>
-    <row r="26" spans="1:66" ht="15.75" thickBot="1">
+    <row r="26" spans="1:71" ht="15.75" thickBot="1">
       <c r="A26" s="94">
         <v>3</v>
       </c>
@@ -6663,7 +6745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:66" ht="15.75" thickBot="1">
+    <row r="27" spans="1:71" ht="15.75" thickBot="1">
       <c r="A27" s="95">
         <v>4</v>
       </c>
@@ -6863,7 +6945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:66" ht="15.75" thickBot="1">
+    <row r="28" spans="1:71" ht="15.75" thickBot="1">
       <c r="A28" s="92">
         <v>1</v>
       </c>
@@ -7063,7 +7145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:66" ht="15.75" thickBot="1">
+    <row r="29" spans="1:71" ht="15.75" thickBot="1">
       <c r="A29" s="93">
         <v>2</v>
       </c>
@@ -7263,7 +7345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:66" ht="15.75" thickBot="1">
+    <row r="30" spans="1:71" ht="15.75" thickBot="1">
       <c r="A30" s="94">
         <v>3</v>
       </c>
@@ -7463,7 +7545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:66" ht="15.75" thickBot="1">
+    <row r="31" spans="1:71" ht="15.75" thickBot="1">
       <c r="A31" s="95">
         <v>4</v>
       </c>
@@ -7663,7 +7745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:66" ht="15.75" thickBot="1">
+    <row r="32" spans="1:71" ht="15.75" thickBot="1">
       <c r="A32" s="92">
         <v>1</v>
       </c>
@@ -14864,7 +14946,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="BP9:BS25"/>
     <mergeCell ref="S1:AH1"/>
     <mergeCell ref="AI1:AX1"/>
     <mergeCell ref="AY1:BN1"/>

</xml_diff>